<commit_message>
updated pom file, added new screenshot
</commit_message>
<xml_diff>
--- a/requiredSource/TestData.xlsx
+++ b/requiredSource/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-8484" yWindow="-1320" windowWidth="21180" windowHeight="5892" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20388" windowHeight="6216" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -185,11 +185,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -568,7 +569,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,7 +599,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>42857</v>
+        <v>42885</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -647,12 +648,13 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -683,7 +685,7 @@
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>29</v>
       </c>
     </row>
@@ -721,7 +723,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,7 +777,7 @@
         <v>26</v>
       </c>
       <c r="B6">
-        <v>123</v>
+        <v>12345</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>